<commit_message>
Added second test where search elements are sorted.
</commit_message>
<xml_diff>
--- a/tests/Performance results.xlsx
+++ b/tests/Performance results.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="normal dist., static" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="normal dist. sorted, static" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>sigma</t>
   </si>
@@ -27,25 +27,25 @@
     <t>std::vector</t>
   </si>
   <si>
-    <t>so::l&lt;count&gt;</t>
+    <t>std::set</t>
   </si>
   <si>
-    <t>so::l&lt;transpose&gt;</t>
+    <t>so::list&lt;count&gt;</t>
   </si>
   <si>
-    <t>so::l&lt;move-to-front&gt;</t>
+    <t>so::list&lt;transpose&gt;</t>
   </si>
   <si>
-    <t>so::v&lt;count&gt;</t>
+    <t>so::list&lt;move-to-front&gt;</t>
   </si>
   <si>
-    <t>so::v&lt;transpose&gt;</t>
+    <t>so::vector&lt;count&gt;</t>
   </si>
   <si>
-    <t>so::v&lt;move-to-front&gt;</t>
+    <t>so::vector&lt;transpose&gt;</t>
   </si>
   <si>
-    <t>std::set</t>
+    <t>so::vector&lt;move-to-front&gt;</t>
   </si>
 </sst>
 </file>
@@ -124,21 +124,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Time to search 100000 normally distributed integers in</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> a static container of 100000 elements by variance</a:t>
+              <a:t>Time to search 100000 normally distributed integers in a static container of 100000 elements by variance</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -239,7 +225,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$C$1</c:f>
+              <c:f>'normal dist., static'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -283,7 +269,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$C$2:$C$8</c:f>
+              <c:f>'normal dist., static'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -318,7 +304,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$D$1</c:f>
+              <c:f>'normal dist., static'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -362,7 +348,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$D$2:$D$8</c:f>
+              <c:f>'normal dist., static'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -397,11 +383,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$E$1</c:f>
+              <c:f>'normal dist., static'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::l&lt;count&gt;</c:v>
+                  <c:v>so::list&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -441,7 +427,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$E$2:$E$8</c:f>
+              <c:f>'normal dist., static'!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -476,11 +462,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$F$1</c:f>
+              <c:f>'normal dist., static'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::l&lt;transpose&gt;</c:v>
+                  <c:v>so::list&lt;transpose&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -520,7 +506,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$F$2:$F$8</c:f>
+              <c:f>'normal dist., static'!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -555,11 +541,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$G$1</c:f>
+              <c:f>'normal dist., static'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::l&lt;move-to-front&gt;</c:v>
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -599,7 +585,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$G$2:$G$8</c:f>
+              <c:f>'normal dist., static'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -634,11 +620,11 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$H$1</c:f>
+              <c:f>'normal dist., static'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::v&lt;count&gt;</c:v>
+                  <c:v>so::vector&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -678,7 +664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$H$2:$H$8</c:f>
+              <c:f>'normal dist., static'!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -713,11 +699,11 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$I$1</c:f>
+              <c:f>'normal dist., static'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::v&lt;transpose&gt;</c:v>
+                  <c:v>so::vector&lt;transpose&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -757,7 +743,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$I$2:$I$8</c:f>
+              <c:f>'normal dist., static'!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -792,11 +778,11 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$J$1</c:f>
+              <c:f>'normal dist., static'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::v&lt;move-to-front&gt;</c:v>
+                  <c:v>so::vector&lt;move-to-front&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -836,7 +822,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$J$2:$J$8</c:f>
+              <c:f>'normal dist., static'!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -975,20 +961,919 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time to search 100000 normally distributed and sorted integers in a static container of 100000 elements by variance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std::set</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std::vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.6339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6030000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std::list</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.592000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.701000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.717000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.872999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;count&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>51.807000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.204000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.074999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.082000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.885</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4860000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8530000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;transpose&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.483000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.388999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.388999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.452</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.483000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.342000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>26.940999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2569999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1840000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95099999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::vector&lt;count&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>51.027000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.338999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.823999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.804000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.887</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.762</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::vector&lt;transpose&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6030000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5720000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal dist. sorted, static'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::vector&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal dist. sorted, static'!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>32.369999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.401000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.824999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.481999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.481999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.684999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="43807872"/>
+        <c:axId val="43809408"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="43807872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sigma</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43809408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43809408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43807872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1120140</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1299,21 +2184,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1321,31 +2207,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1356,28 +2242,28 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="C2">
+        <v>4.7110000000000003</v>
+      </c>
+      <c r="D2">
         <v>10.576000000000001</v>
       </c>
-      <c r="D2">
-        <v>4.7110000000000003</v>
-      </c>
       <c r="E2">
+        <v>31.465</v>
+      </c>
+      <c r="F2">
+        <v>3.5880000000000001</v>
+      </c>
+      <c r="G2">
+        <v>50.341000000000001</v>
+      </c>
+      <c r="H2">
+        <v>43.789000000000001</v>
+      </c>
+      <c r="I2">
+        <v>10.608000000000001</v>
+      </c>
+      <c r="J2">
         <v>49.545000000000002</v>
-      </c>
-      <c r="F2">
-        <v>10.608000000000001</v>
-      </c>
-      <c r="G2">
-        <v>43.789000000000001</v>
-      </c>
-      <c r="H2">
-        <v>50.341000000000001</v>
-      </c>
-      <c r="I2">
-        <v>3.5880000000000001</v>
-      </c>
-      <c r="J2">
-        <v>31.465</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1388,28 +2274,28 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C3">
+        <v>3.5409999999999999</v>
+      </c>
+      <c r="D3">
         <v>10.654</v>
       </c>
-      <c r="D3">
-        <v>3.5409999999999999</v>
-      </c>
       <c r="E3">
+        <v>30.716000000000001</v>
+      </c>
+      <c r="F3">
+        <v>3.5249999999999999</v>
+      </c>
+      <c r="G3">
+        <v>49.872999999999998</v>
+      </c>
+      <c r="H3">
+        <v>32.619</v>
+      </c>
+      <c r="I3">
+        <v>10.202</v>
+      </c>
+      <c r="J3">
         <v>43.118000000000002</v>
-      </c>
-      <c r="F3">
-        <v>10.202</v>
-      </c>
-      <c r="G3">
-        <v>32.619</v>
-      </c>
-      <c r="H3">
-        <v>49.872999999999998</v>
-      </c>
-      <c r="I3">
-        <v>3.5249999999999999</v>
-      </c>
-      <c r="J3">
-        <v>30.716000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1420,28 +2306,28 @@
         <v>3.1E-2</v>
       </c>
       <c r="C4">
+        <v>3.9780000000000002</v>
+      </c>
+      <c r="D4">
         <v>13.54</v>
       </c>
-      <c r="D4">
-        <v>3.9780000000000002</v>
-      </c>
       <c r="E4">
+        <v>34.771999999999998</v>
+      </c>
+      <c r="F4">
+        <v>4.4610000000000003</v>
+      </c>
+      <c r="G4">
+        <v>61.37</v>
+      </c>
+      <c r="H4">
+        <v>21.402999999999999</v>
+      </c>
+      <c r="I4">
+        <v>12.823</v>
+      </c>
+      <c r="J4">
         <v>25.957999999999998</v>
-      </c>
-      <c r="F4">
-        <v>12.823</v>
-      </c>
-      <c r="G4">
-        <v>21.402999999999999</v>
-      </c>
-      <c r="H4">
-        <v>61.37</v>
-      </c>
-      <c r="I4">
-        <v>4.4610000000000003</v>
-      </c>
-      <c r="J4">
-        <v>34.771999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1452,28 +2338,28 @@
         <v>3.1E-2</v>
       </c>
       <c r="C5">
+        <v>5.2720000000000002</v>
+      </c>
+      <c r="D5">
         <v>13.946</v>
       </c>
-      <c r="D5">
-        <v>5.2720000000000002</v>
-      </c>
       <c r="E5">
+        <v>38.531999999999996</v>
+      </c>
+      <c r="F5">
+        <v>4.5860000000000003</v>
+      </c>
+      <c r="G5">
+        <v>66.19</v>
+      </c>
+      <c r="H5">
+        <v>18.86</v>
+      </c>
+      <c r="I5">
+        <v>14.461</v>
+      </c>
+      <c r="J5">
         <v>21.762</v>
-      </c>
-      <c r="F5">
-        <v>14.461</v>
-      </c>
-      <c r="G5">
-        <v>18.86</v>
-      </c>
-      <c r="H5">
-        <v>66.19</v>
-      </c>
-      <c r="I5">
-        <v>4.5860000000000003</v>
-      </c>
-      <c r="J5">
-        <v>38.531999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1484,28 +2370,28 @@
         <v>3.1E-2</v>
       </c>
       <c r="C6">
+        <v>3.7749999999999999</v>
+      </c>
+      <c r="D6">
         <v>10.81</v>
       </c>
-      <c r="D6">
-        <v>3.7749999999999999</v>
-      </c>
       <c r="E6">
+        <v>30.201000000000001</v>
+      </c>
+      <c r="F6">
+        <v>3.556</v>
+      </c>
+      <c r="G6">
+        <v>52.494999999999997</v>
+      </c>
+      <c r="H6">
+        <v>11.606</v>
+      </c>
+      <c r="I6">
+        <v>10.654</v>
+      </c>
+      <c r="J6">
         <v>14.976000000000001</v>
-      </c>
-      <c r="F6">
-        <v>10.654</v>
-      </c>
-      <c r="G6">
-        <v>11.606</v>
-      </c>
-      <c r="H6">
-        <v>52.494999999999997</v>
-      </c>
-      <c r="I6">
-        <v>3.556</v>
-      </c>
-      <c r="J6">
-        <v>30.201000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1516,28 +2402,28 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C7">
+        <v>4.0709999999999997</v>
+      </c>
+      <c r="D7">
         <v>10.965999999999999</v>
       </c>
-      <c r="D7">
-        <v>4.0709999999999997</v>
-      </c>
       <c r="E7">
+        <v>31.73</v>
+      </c>
+      <c r="F7">
+        <v>3.6659999999999999</v>
+      </c>
+      <c r="G7">
+        <v>54.146999999999998</v>
+      </c>
+      <c r="H7">
+        <v>7.6589999999999998</v>
+      </c>
+      <c r="I7">
+        <v>10.779</v>
+      </c>
+      <c r="J7">
         <v>9.2349999999999994</v>
-      </c>
-      <c r="F7">
-        <v>10.779</v>
-      </c>
-      <c r="G7">
-        <v>7.6589999999999998</v>
-      </c>
-      <c r="H7">
-        <v>54.146999999999998</v>
-      </c>
-      <c r="I7">
-        <v>3.6659999999999999</v>
-      </c>
-      <c r="J7">
-        <v>31.73</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1548,28 +2434,28 @@
         <v>3.1E-2</v>
       </c>
       <c r="C8">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="D8">
         <v>11.013</v>
       </c>
-      <c r="D8">
-        <v>3.6190000000000002</v>
-      </c>
       <c r="E8">
+        <v>30.824999999999999</v>
+      </c>
+      <c r="F8">
+        <v>3.6970000000000001</v>
+      </c>
+      <c r="G8">
+        <v>51.48</v>
+      </c>
+      <c r="H8">
+        <v>3.0569999999999999</v>
+      </c>
+      <c r="I8">
+        <v>10.576000000000001</v>
+      </c>
+      <c r="J8">
         <v>4.0869999999999997</v>
-      </c>
-      <c r="F8">
-        <v>10.576000000000001</v>
-      </c>
-      <c r="G8">
-        <v>3.0569999999999999</v>
-      </c>
-      <c r="H8">
-        <v>51.48</v>
-      </c>
-      <c r="I8">
-        <v>3.6970000000000001</v>
-      </c>
-      <c r="J8">
-        <v>30.824999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1581,13 +2467,285 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>15000</v>
+      </c>
+      <c r="B2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>3.6339999999999999</v>
+      </c>
+      <c r="D2">
+        <v>10.592000000000001</v>
+      </c>
+      <c r="E2">
+        <v>32.369999999999997</v>
+      </c>
+      <c r="F2">
+        <v>3.65</v>
+      </c>
+      <c r="G2">
+        <v>51.027000000000001</v>
+      </c>
+      <c r="H2">
+        <v>26.940999999999999</v>
+      </c>
+      <c r="I2">
+        <v>10.545</v>
+      </c>
+      <c r="J2">
+        <v>51.807000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>3.806</v>
+      </c>
+      <c r="D3">
+        <v>11.185</v>
+      </c>
+      <c r="E3">
+        <v>32.401000000000003</v>
+      </c>
+      <c r="F3">
+        <v>3.79</v>
+      </c>
+      <c r="G3">
+        <v>51.338999999999999</v>
+      </c>
+      <c r="H3">
+        <v>17.55</v>
+      </c>
+      <c r="I3">
+        <v>10.483000000000001</v>
+      </c>
+      <c r="J3">
+        <v>38.204000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5000</v>
+      </c>
+      <c r="B4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>3.9</v>
+      </c>
+      <c r="D4">
+        <v>10.92</v>
+      </c>
+      <c r="E4">
+        <v>30.824999999999999</v>
+      </c>
+      <c r="F4">
+        <v>3.5720000000000001</v>
+      </c>
+      <c r="G4">
+        <v>50.823999999999998</v>
+      </c>
+      <c r="H4">
+        <v>7.0350000000000001</v>
+      </c>
+      <c r="I4">
+        <v>10.388999999999999</v>
+      </c>
+      <c r="J4">
+        <v>21.074999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4000</v>
+      </c>
+      <c r="B5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C5">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="D5">
+        <v>10.701000000000001</v>
+      </c>
+      <c r="E5">
+        <v>30.481999999999999</v>
+      </c>
+      <c r="F5">
+        <v>3.6030000000000002</v>
+      </c>
+      <c r="G5">
+        <v>50.804000000000002</v>
+      </c>
+      <c r="H5">
+        <v>5.2569999999999997</v>
+      </c>
+      <c r="I5">
+        <v>10.388999999999999</v>
+      </c>
+      <c r="J5">
+        <v>17.082000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3000</v>
+      </c>
+      <c r="B6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>3.6659999999999999</v>
+      </c>
+      <c r="D6">
+        <v>10.717000000000001</v>
+      </c>
+      <c r="E6">
+        <v>30.7</v>
+      </c>
+      <c r="F6">
+        <v>3.65</v>
+      </c>
+      <c r="G6">
+        <v>50.887</v>
+      </c>
+      <c r="H6">
+        <v>3.6659999999999999</v>
+      </c>
+      <c r="I6">
+        <v>10.452</v>
+      </c>
+      <c r="J6">
+        <v>12.885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2000</v>
+      </c>
+      <c r="B7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.6970000000000001</v>
+      </c>
+      <c r="D7">
+        <v>10.81</v>
+      </c>
+      <c r="E7">
+        <v>30.481999999999999</v>
+      </c>
+      <c r="F7">
+        <v>3.65</v>
+      </c>
+      <c r="G7">
+        <v>50.762</v>
+      </c>
+      <c r="H7">
+        <v>2.1840000000000002</v>
+      </c>
+      <c r="I7">
+        <v>10.483000000000001</v>
+      </c>
+      <c r="J7">
+        <v>8.4860000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>3.6030000000000002</v>
+      </c>
+      <c r="D8">
+        <v>10.872999999999999</v>
+      </c>
+      <c r="E8">
+        <v>30.684999999999999</v>
+      </c>
+      <c r="F8">
+        <v>3.5720000000000001</v>
+      </c>
+      <c r="G8">
+        <v>50.98</v>
+      </c>
+      <c r="H8">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="I8">
+        <v>10.342000000000001</v>
+      </c>
+      <c r="J8">
+        <v>3.8530000000000002</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Going in a different direction with the second half of the performance tests. This is a point check-in of what I have now just so I don't lose it.
</commit_message>
<xml_diff>
--- a/tests/Performance results.xlsx
+++ b/tests/Performance results.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
-    <sheet name="normal dist., static" sheetId="1" r:id="rId1"/>
-    <sheet name="normal dist. sorted, static" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="normal" sheetId="1" r:id="rId1"/>
+    <sheet name="normal, sorted" sheetId="2" r:id="rId2"/>
+    <sheet name="geometric, 100000" sheetId="3" r:id="rId3"/>
+    <sheet name="geometric, 1000000" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>sigma</t>
   </si>
@@ -33,19 +34,25 @@
     <t>so::list&lt;count&gt;</t>
   </si>
   <si>
-    <t>so::list&lt;transpose&gt;</t>
-  </si>
-  <si>
     <t>so::list&lt;move-to-front&gt;</t>
   </si>
   <si>
     <t>so::vector&lt;count&gt;</t>
   </si>
   <si>
-    <t>so::vector&lt;transpose&gt;</t>
+    <t>so::vector&lt;move-to-front&gt;</t>
   </si>
   <si>
-    <t>so::vector&lt;move-to-front&gt;</t>
+    <t>param</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>so::list&lt;transpose&gt;</t>
+  </si>
+  <si>
+    <t>so::vector&lt;transpose&gt;</t>
   </si>
 </sst>
 </file>
@@ -124,7 +131,19 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Time to search 100000 normally distributed integers in a static container of 100000 elements by variance</a:t>
+              <a:t>Time to construct a </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>container of 100000 elements and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>search 100000 normally distributed integers,  by variance</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -146,7 +165,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$B$1</c:f>
+              <c:f>normal!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -160,7 +179,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -190,30 +209,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$B$2:$B$8</c:f>
+              <c:f>normal!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.5999999999999999E-2</c:v>
+                  <c:v>6.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>5.7000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -221,11 +240,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$D$1</c:f>
+              <c:f>normal!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -239,7 +258,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -269,30 +288,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$D$2:$D$8</c:f>
+              <c:f>normal!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10.576000000000001</c:v>
+                  <c:v>11.378</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.654</c:v>
+                  <c:v>11.632</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.54</c:v>
+                  <c:v>11.818</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.946</c:v>
+                  <c:v>11.241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.81</c:v>
+                  <c:v>11.202999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.965999999999999</c:v>
+                  <c:v>11.497999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.013</c:v>
+                  <c:v>11.571999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -300,11 +319,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$C$1</c:f>
+              <c:f>normal!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -318,7 +337,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -348,30 +367,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$C$2:$C$8</c:f>
+              <c:f>normal!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.7110000000000003</c:v>
+                  <c:v>3.9369999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5409999999999999</c:v>
+                  <c:v>4.0209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9780000000000002</c:v>
+                  <c:v>3.9630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2720000000000002</c:v>
+                  <c:v>3.802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.7749999999999999</c:v>
+                  <c:v>3.827</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0709999999999997</c:v>
+                  <c:v>3.8210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6190000000000002</c:v>
+                  <c:v>3.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -379,11 +398,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="8"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$J$1</c:f>
+              <c:f>normal!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -397,7 +416,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -427,30 +446,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$J$2:$J$8</c:f>
+              <c:f>normal!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>49.545000000000002</c:v>
+                  <c:v>54.085999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.118000000000002</c:v>
+                  <c:v>41.878</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.957999999999998</c:v>
+                  <c:v>22.771999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.762</c:v>
+                  <c:v>18.327999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.976000000000001</c:v>
+                  <c:v>14.242000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.2349999999999994</c:v>
+                  <c:v>9.2910000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0869999999999997</c:v>
+                  <c:v>4.2460000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,11 +477,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="7"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$I$1</c:f>
+              <c:f>normal!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -476,7 +495,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -506,30 +525,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$I$2:$I$8</c:f>
+              <c:f>normal!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10.608000000000001</c:v>
+                  <c:v>11.423999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.202</c:v>
+                  <c:v>11.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.823</c:v>
+                  <c:v>11.204000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.461</c:v>
+                  <c:v>11.444000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.654</c:v>
+                  <c:v>11.212999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.779</c:v>
+                  <c:v>11.215999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.576000000000001</c:v>
+                  <c:v>11.117000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,11 +556,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="6"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$H$1</c:f>
+              <c:f>normal!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -555,7 +574,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -585,30 +604,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$H$2:$H$8</c:f>
+              <c:f>normal!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>43.789000000000001</c:v>
+                  <c:v>47.075000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.619</c:v>
+                  <c:v>35.542000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.402999999999999</c:v>
+                  <c:v>20.009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.86</c:v>
+                  <c:v>16.239999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.606</c:v>
+                  <c:v>12.122</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.6589999999999998</c:v>
+                  <c:v>7.8540000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0569999999999999</c:v>
+                  <c:v>3.1139999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,11 +635,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="4"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$G$1</c:f>
+              <c:f>normal!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -634,7 +653,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -664,30 +683,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$G$2:$G$8</c:f>
+              <c:f>normal!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>50.341000000000001</c:v>
+                  <c:v>55.220999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.872999999999998</c:v>
+                  <c:v>56.359000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.37</c:v>
+                  <c:v>54.023000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.19</c:v>
+                  <c:v>54.268999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.494999999999997</c:v>
+                  <c:v>54.198999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.146999999999998</c:v>
+                  <c:v>54.587000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51.48</c:v>
+                  <c:v>54.194000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,11 +714,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
+          <c:idx val="3"/>
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$F$1</c:f>
+              <c:f>normal!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -713,7 +732,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -743,30 +762,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$F$2:$F$8</c:f>
+              <c:f>normal!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.5880000000000001</c:v>
+                  <c:v>3.8639999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5249999999999999</c:v>
+                  <c:v>3.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4610000000000003</c:v>
+                  <c:v>3.8370000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5860000000000003</c:v>
+                  <c:v>3.843</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.556</c:v>
+                  <c:v>3.8620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6659999999999999</c:v>
+                  <c:v>3.827</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6970000000000001</c:v>
+                  <c:v>3.8370000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -774,11 +793,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
+          <c:idx val="2"/>
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist., static'!$E$1</c:f>
+              <c:f>normal!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -792,7 +811,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist., static'!$A$2:$A$8</c:f>
+              <c:f>normal!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -822,30 +841,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist., static'!$E$2:$E$8</c:f>
+              <c:f>normal!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>31.465</c:v>
+                  <c:v>35.305</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.716000000000001</c:v>
+                  <c:v>34.494999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.771999999999998</c:v>
+                  <c:v>33.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.531999999999996</c:v>
+                  <c:v>32.822000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.201000000000001</c:v>
+                  <c:v>32.838000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.73</c:v>
+                  <c:v>32.896999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.824999999999999</c:v>
+                  <c:v>32.622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -862,11 +881,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113844992"/>
-        <c:axId val="113846912"/>
+        <c:axId val="112877952"/>
+        <c:axId val="112879872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113844992"/>
+        <c:axId val="112877952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113846912"/>
+        <c:crossAx val="112879872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -903,7 +922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113846912"/>
+        <c:axId val="112879872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113844992"/>
+        <c:crossAx val="112877952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -988,7 +1007,19 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Time to search 100000 normally distributed and sorted integers in a static container of 100000 elements by variance</a:t>
+              <a:t>Time to construct </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>a container of 100000 elements and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>search 100000 normally distributed and sorted integers, by variance</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -1010,7 +1041,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$B$1</c:f>
+              <c:f>'normal, sorted'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1024,7 +1055,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1054,30 +1085,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$B$2:$B$8</c:f>
+              <c:f>'normal, sorted'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>5.0999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>4.9000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>4.7E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>4.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>4.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1089,11 +1120,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$C$1</c:f>
+              <c:f>'normal, sorted'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std::vector</c:v>
+                  <c:v>std::list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1103,7 +1134,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1133,30 +1164,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$C$2:$C$8</c:f>
+              <c:f>'normal, sorted'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.6339999999999999</c:v>
+                  <c:v>11.887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.806</c:v>
+                  <c:v>11.209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9</c:v>
+                  <c:v>11.212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6190000000000002</c:v>
+                  <c:v>11.839</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6659999999999999</c:v>
+                  <c:v>11.592000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6970000000000001</c:v>
+                  <c:v>11.558999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6030000000000002</c:v>
+                  <c:v>11.135999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,11 +1199,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$D$1</c:f>
+              <c:f>'normal, sorted'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std::list</c:v>
+                  <c:v>std::vector</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1182,7 +1213,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1212,30 +1243,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$D$2:$D$8</c:f>
+              <c:f>'normal, sorted'!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10.592000000000001</c:v>
+                  <c:v>4.0179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.185</c:v>
+                  <c:v>3.8980000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.92</c:v>
+                  <c:v>4.048</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.701000000000001</c:v>
+                  <c:v>3.8260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.717000000000001</c:v>
+                  <c:v>4.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.81</c:v>
+                  <c:v>3.8180000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.872999999999999</c:v>
+                  <c:v>3.7869999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1243,11 +1274,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="9"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$J$1</c:f>
+              <c:f>'normal, sorted'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1261,7 +1292,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1291,30 +1322,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$J$2:$J$8</c:f>
+              <c:f>'normal, sorted'!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>51.807000000000002</c:v>
+                  <c:v>56.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.204000000000001</c:v>
+                  <c:v>40.884999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.074999999999999</c:v>
+                  <c:v>22.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.082000000000001</c:v>
+                  <c:v>18.146999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.885</c:v>
+                  <c:v>14.667999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4860000000000007</c:v>
+                  <c:v>9.1419999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8530000000000002</c:v>
+                  <c:v>4.0439999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,11 +1353,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
+          <c:idx val="3"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$I$1</c:f>
+              <c:f>'normal, sorted'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1340,7 +1371,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1370,30 +1401,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$I$2:$I$8</c:f>
+              <c:f>'normal, sorted'!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10.545</c:v>
+                  <c:v>11.587999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.483000000000001</c:v>
+                  <c:v>11.715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.388999999999999</c:v>
+                  <c:v>11.677</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.388999999999999</c:v>
+                  <c:v>11.677</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.452</c:v>
+                  <c:v>11.624000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.483000000000001</c:v>
+                  <c:v>11.289</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.342000000000001</c:v>
+                  <c:v>10.954000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,11 +1432,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="8"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$H$1</c:f>
+              <c:f>'normal, sorted'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1419,7 +1450,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1449,30 +1480,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$H$2:$H$8</c:f>
+              <c:f>'normal, sorted'!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>26.940999999999999</c:v>
+                  <c:v>29.841000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.55</c:v>
+                  <c:v>18.516999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0350000000000001</c:v>
+                  <c:v>8.2110000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2569999999999997</c:v>
+                  <c:v>5.7130000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6659999999999999</c:v>
+                  <c:v>3.8650000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1840000000000002</c:v>
+                  <c:v>2.2370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.95099999999999996</c:v>
+                  <c:v>0.98799999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1480,11 +1511,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
+          <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$G$1</c:f>
+              <c:f>'normal, sorted'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1498,7 +1529,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1528,30 +1559,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$G$2:$G$8</c:f>
+              <c:f>'normal, sorted'!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>51.027000000000001</c:v>
+                  <c:v>54.564999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.338999999999999</c:v>
+                  <c:v>54.441000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.823999999999998</c:v>
+                  <c:v>57.148000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.804000000000002</c:v>
+                  <c:v>54.430999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.887</c:v>
+                  <c:v>53.585999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.762</c:v>
+                  <c:v>53.823999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.98</c:v>
+                  <c:v>54.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,11 +1590,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$F$1</c:f>
+              <c:f>'normal, sorted'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1577,7 +1608,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1607,30 +1638,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$F$2:$F$8</c:f>
+              <c:f>'normal, sorted'!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.65</c:v>
+                  <c:v>3.883</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.79</c:v>
+                  <c:v>3.9279999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5720000000000001</c:v>
+                  <c:v>3.8969999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6030000000000002</c:v>
+                  <c:v>3.7370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.65</c:v>
+                  <c:v>3.7549999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.65</c:v>
+                  <c:v>3.7480000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5720000000000001</c:v>
+                  <c:v>3.7410000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1638,11 +1669,11 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="9"/>
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'normal dist. sorted, static'!$E$1</c:f>
+              <c:f>'normal, sorted'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1656,7 +1687,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$A$2:$A$8</c:f>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1686,30 +1717,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'normal dist. sorted, static'!$E$2:$E$8</c:f>
+              <c:f>'normal, sorted'!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>32.369999999999997</c:v>
+                  <c:v>33.569000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.401000000000003</c:v>
+                  <c:v>33.481999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.824999999999999</c:v>
+                  <c:v>35.371000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.481999999999999</c:v>
+                  <c:v>34.941000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.7</c:v>
+                  <c:v>33.081000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.481999999999999</c:v>
+                  <c:v>33.090000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.684999999999999</c:v>
+                  <c:v>32.238999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1726,11 +1757,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43807872"/>
-        <c:axId val="43809408"/>
+        <c:axId val="114120192"/>
+        <c:axId val="114122112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43807872"/>
+        <c:axId val="114120192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1759,7 +1790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43809408"/>
+        <c:crossAx val="114122112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1767,7 +1798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43809408"/>
+        <c:axId val="114122112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1797,7 +1828,1255 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43807872"/>
+        <c:crossAx val="114120192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time to construct </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>a container of 100000 elements and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>search 100000 geometrically distributed integers, by </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="1" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>p</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" i="1">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 100000'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std::set</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 100000'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;count&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$C$2:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>269</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 100000'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="115246976"/>
+        <c:axId val="115249152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="115246976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" i="1"/>
+                  <a:t>p</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115249152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="115249152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115246976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time to construct </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>a container of 1000000 elements and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>search 100000 geometrically distributed integers in, by </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="1" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>p</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 1000000'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>std::set</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>692</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>682</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>681</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>707</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 1000000'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;count&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$C$2:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>623</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>792</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1124</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 1000000'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="116414720"/>
+        <c:axId val="116425088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="116414720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" i="1"/>
+                  <a:t>p</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="116425088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="116425088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="116414720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1835,15 +3114,17 @@
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1870,10 +3151,82 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1120140</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>868680</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>26670</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>331470</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2184,22 +3537,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -2210,28 +3562,28 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2239,31 +3591,31 @@
         <v>15000</v>
       </c>
       <c r="B2">
-        <v>4.5999999999999999E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="C2">
-        <v>4.7110000000000003</v>
+        <v>11.378</v>
       </c>
       <c r="D2">
-        <v>10.576000000000001</v>
+        <v>3.9369999999999998</v>
       </c>
       <c r="E2">
-        <v>31.465</v>
+        <v>54.085999999999999</v>
       </c>
       <c r="F2">
-        <v>3.5880000000000001</v>
+        <v>11.423999999999999</v>
       </c>
       <c r="G2">
-        <v>50.341000000000001</v>
+        <v>47.075000000000003</v>
       </c>
       <c r="H2">
-        <v>43.789000000000001</v>
+        <v>55.220999999999997</v>
       </c>
       <c r="I2">
-        <v>10.608000000000001</v>
+        <v>3.8639999999999999</v>
       </c>
       <c r="J2">
-        <v>49.545000000000002</v>
+        <v>35.305</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2271,31 +3623,31 @@
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>1.4999999999999999E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C3">
-        <v>3.5409999999999999</v>
+        <v>11.632</v>
       </c>
       <c r="D3">
-        <v>10.654</v>
+        <v>4.0209999999999999</v>
       </c>
       <c r="E3">
-        <v>30.716000000000001</v>
+        <v>41.878</v>
       </c>
       <c r="F3">
-        <v>3.5249999999999999</v>
+        <v>11.78</v>
       </c>
       <c r="G3">
-        <v>49.872999999999998</v>
+        <v>35.542000000000002</v>
       </c>
       <c r="H3">
-        <v>32.619</v>
+        <v>56.359000000000002</v>
       </c>
       <c r="I3">
-        <v>10.202</v>
+        <v>3.92</v>
       </c>
       <c r="J3">
-        <v>43.118000000000002</v>
+        <v>34.494999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2303,31 +3655,31 @@
         <v>5000</v>
       </c>
       <c r="B4">
-        <v>3.1E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C4">
-        <v>3.9780000000000002</v>
+        <v>11.818</v>
       </c>
       <c r="D4">
-        <v>13.54</v>
+        <v>3.9630000000000001</v>
       </c>
       <c r="E4">
-        <v>34.771999999999998</v>
+        <v>22.771999999999998</v>
       </c>
       <c r="F4">
-        <v>4.4610000000000003</v>
+        <v>11.204000000000001</v>
       </c>
       <c r="G4">
-        <v>61.37</v>
+        <v>20.009</v>
       </c>
       <c r="H4">
-        <v>21.402999999999999</v>
+        <v>54.023000000000003</v>
       </c>
       <c r="I4">
-        <v>12.823</v>
+        <v>3.8370000000000002</v>
       </c>
       <c r="J4">
-        <v>25.957999999999998</v>
+        <v>33.44</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2335,31 +3687,31 @@
         <v>4000</v>
       </c>
       <c r="B5">
-        <v>3.1E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C5">
-        <v>5.2720000000000002</v>
+        <v>11.241</v>
       </c>
       <c r="D5">
-        <v>13.946</v>
+        <v>3.802</v>
       </c>
       <c r="E5">
-        <v>38.531999999999996</v>
+        <v>18.327999999999999</v>
       </c>
       <c r="F5">
-        <v>4.5860000000000003</v>
+        <v>11.444000000000001</v>
       </c>
       <c r="G5">
-        <v>66.19</v>
+        <v>16.239999999999998</v>
       </c>
       <c r="H5">
-        <v>18.86</v>
+        <v>54.268999999999998</v>
       </c>
       <c r="I5">
-        <v>14.461</v>
+        <v>3.843</v>
       </c>
       <c r="J5">
-        <v>21.762</v>
+        <v>32.822000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2367,31 +3719,31 @@
         <v>3000</v>
       </c>
       <c r="B6">
-        <v>3.1E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="C6">
-        <v>3.7749999999999999</v>
+        <v>11.202999999999999</v>
       </c>
       <c r="D6">
-        <v>10.81</v>
+        <v>3.827</v>
       </c>
       <c r="E6">
-        <v>30.201000000000001</v>
+        <v>14.242000000000001</v>
       </c>
       <c r="F6">
-        <v>3.556</v>
+        <v>11.212999999999999</v>
       </c>
       <c r="G6">
-        <v>52.494999999999997</v>
+        <v>12.122</v>
       </c>
       <c r="H6">
-        <v>11.606</v>
+        <v>54.198999999999998</v>
       </c>
       <c r="I6">
-        <v>10.654</v>
+        <v>3.8620000000000001</v>
       </c>
       <c r="J6">
-        <v>14.976000000000001</v>
+        <v>32.838000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2399,31 +3751,31 @@
         <v>2000</v>
       </c>
       <c r="B7">
-        <v>1.4999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C7">
-        <v>4.0709999999999997</v>
+        <v>11.497999999999999</v>
       </c>
       <c r="D7">
-        <v>10.965999999999999</v>
+        <v>3.8210000000000002</v>
       </c>
       <c r="E7">
-        <v>31.73</v>
+        <v>9.2910000000000004</v>
       </c>
       <c r="F7">
-        <v>3.6659999999999999</v>
+        <v>11.215999999999999</v>
       </c>
       <c r="G7">
-        <v>54.146999999999998</v>
+        <v>7.8540000000000001</v>
       </c>
       <c r="H7">
-        <v>7.6589999999999998</v>
+        <v>54.587000000000003</v>
       </c>
       <c r="I7">
-        <v>10.779</v>
+        <v>3.827</v>
       </c>
       <c r="J7">
-        <v>9.2349999999999994</v>
+        <v>32.896999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2431,31 +3783,31 @@
         <v>1000</v>
       </c>
       <c r="B8">
-        <v>3.1E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C8">
-        <v>3.6190000000000002</v>
+        <v>11.571999999999999</v>
       </c>
       <c r="D8">
-        <v>11.013</v>
+        <v>3.84</v>
       </c>
       <c r="E8">
-        <v>30.824999999999999</v>
+        <v>4.2460000000000004</v>
       </c>
       <c r="F8">
-        <v>3.6970000000000001</v>
+        <v>11.117000000000001</v>
       </c>
       <c r="G8">
-        <v>51.48</v>
+        <v>3.1139999999999999</v>
       </c>
       <c r="H8">
-        <v>3.0569999999999999</v>
+        <v>54.194000000000003</v>
       </c>
       <c r="I8">
-        <v>10.576000000000001</v>
+        <v>3.8370000000000002</v>
       </c>
       <c r="J8">
-        <v>4.0869999999999997</v>
+        <v>32.622</v>
       </c>
     </row>
   </sheetData>
@@ -2469,54 +3821,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2524,31 +3875,31 @@
         <v>15000</v>
       </c>
       <c r="B2">
-        <v>1.4999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="C2">
-        <v>3.6339999999999999</v>
+        <v>11.887</v>
       </c>
       <c r="D2">
-        <v>10.592000000000001</v>
+        <v>4.0179999999999998</v>
       </c>
       <c r="E2">
-        <v>32.369999999999997</v>
+        <v>56.33</v>
       </c>
       <c r="F2">
-        <v>3.65</v>
+        <v>11.587999999999999</v>
       </c>
       <c r="G2">
-        <v>51.027000000000001</v>
+        <v>29.841000000000001</v>
       </c>
       <c r="H2">
-        <v>26.940999999999999</v>
+        <v>54.564999999999998</v>
       </c>
       <c r="I2">
-        <v>10.545</v>
+        <v>3.883</v>
       </c>
       <c r="J2">
-        <v>51.807000000000002</v>
+        <v>33.569000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2556,31 +3907,31 @@
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>1.4999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C3">
-        <v>3.806</v>
+        <v>11.209</v>
       </c>
       <c r="D3">
-        <v>11.185</v>
+        <v>3.8980000000000001</v>
       </c>
       <c r="E3">
-        <v>32.401000000000003</v>
+        <v>40.884999999999998</v>
       </c>
       <c r="F3">
-        <v>3.79</v>
+        <v>11.715</v>
       </c>
       <c r="G3">
-        <v>51.338999999999999</v>
+        <v>18.516999999999999</v>
       </c>
       <c r="H3">
-        <v>17.55</v>
+        <v>54.441000000000003</v>
       </c>
       <c r="I3">
-        <v>10.483000000000001</v>
+        <v>3.9279999999999999</v>
       </c>
       <c r="J3">
-        <v>38.204000000000001</v>
+        <v>33.481999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2588,31 +3939,31 @@
         <v>5000</v>
       </c>
       <c r="B4">
-        <v>1.4999999999999999E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="C4">
-        <v>3.9</v>
+        <v>11.212</v>
       </c>
       <c r="D4">
-        <v>10.92</v>
+        <v>4.048</v>
       </c>
       <c r="E4">
-        <v>30.824999999999999</v>
+        <v>22.97</v>
       </c>
       <c r="F4">
-        <v>3.5720000000000001</v>
+        <v>11.677</v>
       </c>
       <c r="G4">
-        <v>50.823999999999998</v>
+        <v>8.2110000000000003</v>
       </c>
       <c r="H4">
-        <v>7.0350000000000001</v>
+        <v>57.148000000000003</v>
       </c>
       <c r="I4">
-        <v>10.388999999999999</v>
+        <v>3.8969999999999998</v>
       </c>
       <c r="J4">
-        <v>21.074999999999999</v>
+        <v>35.371000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2620,31 +3971,31 @@
         <v>4000</v>
       </c>
       <c r="B5">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C5">
-        <v>3.6190000000000002</v>
+        <v>11.839</v>
       </c>
       <c r="D5">
-        <v>10.701000000000001</v>
+        <v>3.8260000000000001</v>
       </c>
       <c r="E5">
-        <v>30.481999999999999</v>
+        <v>18.146999999999998</v>
       </c>
       <c r="F5">
-        <v>3.6030000000000002</v>
+        <v>11.677</v>
       </c>
       <c r="G5">
-        <v>50.804000000000002</v>
+        <v>5.7130000000000001</v>
       </c>
       <c r="H5">
-        <v>5.2569999999999997</v>
+        <v>54.430999999999997</v>
       </c>
       <c r="I5">
-        <v>10.388999999999999</v>
+        <v>3.7370000000000001</v>
       </c>
       <c r="J5">
-        <v>17.082000000000001</v>
+        <v>34.941000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2652,31 +4003,31 @@
         <v>3000</v>
       </c>
       <c r="B6">
-        <v>1.4999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C6">
-        <v>3.6659999999999999</v>
+        <v>11.592000000000001</v>
       </c>
       <c r="D6">
-        <v>10.717000000000001</v>
+        <v>4.1749999999999998</v>
       </c>
       <c r="E6">
-        <v>30.7</v>
+        <v>14.667999999999999</v>
       </c>
       <c r="F6">
-        <v>3.65</v>
+        <v>11.624000000000001</v>
       </c>
       <c r="G6">
-        <v>50.887</v>
+        <v>3.8650000000000002</v>
       </c>
       <c r="H6">
-        <v>3.6659999999999999</v>
+        <v>53.585999999999999</v>
       </c>
       <c r="I6">
-        <v>10.452</v>
+        <v>3.7549999999999999</v>
       </c>
       <c r="J6">
-        <v>12.885</v>
+        <v>33.081000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2684,31 +4035,31 @@
         <v>2000</v>
       </c>
       <c r="B7">
-        <v>1.4999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C7">
-        <v>3.6970000000000001</v>
+        <v>11.558999999999999</v>
       </c>
       <c r="D7">
-        <v>10.81</v>
+        <v>3.8180000000000001</v>
       </c>
       <c r="E7">
-        <v>30.481999999999999</v>
+        <v>9.1419999999999995</v>
       </c>
       <c r="F7">
-        <v>3.65</v>
+        <v>11.289</v>
       </c>
       <c r="G7">
-        <v>50.762</v>
+        <v>2.2370000000000001</v>
       </c>
       <c r="H7">
-        <v>2.1840000000000002</v>
+        <v>53.823999999999998</v>
       </c>
       <c r="I7">
-        <v>10.483000000000001</v>
+        <v>3.7480000000000002</v>
       </c>
       <c r="J7">
-        <v>8.4860000000000007</v>
+        <v>33.090000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2716,31 +4067,31 @@
         <v>1000</v>
       </c>
       <c r="B8">
-        <v>1.4999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C8">
-        <v>3.6030000000000002</v>
+        <v>11.135999999999999</v>
       </c>
       <c r="D8">
-        <v>10.872999999999999</v>
+        <v>3.7869999999999999</v>
       </c>
       <c r="E8">
-        <v>30.684999999999999</v>
+        <v>4.0439999999999996</v>
       </c>
       <c r="F8">
-        <v>3.5720000000000001</v>
+        <v>10.954000000000001</v>
       </c>
       <c r="G8">
-        <v>50.98</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="H8">
-        <v>0.95099999999999996</v>
+        <v>54.33</v>
       </c>
       <c r="I8">
-        <v>10.342000000000001</v>
+        <v>3.7410000000000001</v>
       </c>
       <c r="J8">
-        <v>3.8530000000000002</v>
+        <v>32.238999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2751,12 +4102,604 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.9</v>
+      </c>
+      <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.8</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.7</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.6</v>
+      </c>
+      <c r="B6">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <v>41</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.2</v>
+      </c>
+      <c r="B10">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.1</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.09</v>
+      </c>
+      <c r="B12">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.08</v>
+      </c>
+      <c r="B13">
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B14">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.06</v>
+      </c>
+      <c r="B15">
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>52</v>
+      </c>
+      <c r="D15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.05</v>
+      </c>
+      <c r="B16">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.04</v>
+      </c>
+      <c r="B17">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.03</v>
+      </c>
+      <c r="B18">
+        <v>47</v>
+      </c>
+      <c r="C18">
+        <v>104</v>
+      </c>
+      <c r="D18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.02</v>
+      </c>
+      <c r="B19">
+        <v>43</v>
+      </c>
+      <c r="C19">
+        <v>131</v>
+      </c>
+      <c r="D19">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.01</v>
+      </c>
+      <c r="B20">
+        <v>47</v>
+      </c>
+      <c r="C20">
+        <v>269</v>
+      </c>
+      <c r="D20">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>687</v>
+      </c>
+      <c r="C2">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.9</v>
+      </c>
+      <c r="B3">
+        <v>692</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+      <c r="D3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.8</v>
+      </c>
+      <c r="B4">
+        <v>669</v>
+      </c>
+      <c r="C4">
+        <v>87</v>
+      </c>
+      <c r="D4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.7</v>
+      </c>
+      <c r="B5">
+        <v>689</v>
+      </c>
+      <c r="C5">
+        <v>93</v>
+      </c>
+      <c r="D5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.6</v>
+      </c>
+      <c r="B6">
+        <v>682</v>
+      </c>
+      <c r="C6">
+        <v>107</v>
+      </c>
+      <c r="D6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>743</v>
+      </c>
+      <c r="C7">
+        <v>122</v>
+      </c>
+      <c r="D7">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>704</v>
+      </c>
+      <c r="C8">
+        <v>133</v>
+      </c>
+      <c r="D8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <v>697</v>
+      </c>
+      <c r="C9">
+        <v>135</v>
+      </c>
+      <c r="D9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.2</v>
+      </c>
+      <c r="B10">
+        <v>702</v>
+      </c>
+      <c r="C10">
+        <v>184</v>
+      </c>
+      <c r="D10">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.1</v>
+      </c>
+      <c r="B11">
+        <v>679</v>
+      </c>
+      <c r="C11">
+        <v>282</v>
+      </c>
+      <c r="D11">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.09</v>
+      </c>
+      <c r="B12">
+        <v>700</v>
+      </c>
+      <c r="C12">
+        <v>308</v>
+      </c>
+      <c r="D12">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.08</v>
+      </c>
+      <c r="B13">
+        <v>700</v>
+      </c>
+      <c r="C13">
+        <v>362</v>
+      </c>
+      <c r="D13">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B14">
+        <v>721</v>
+      </c>
+      <c r="C14">
+        <v>399</v>
+      </c>
+      <c r="D14">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.06</v>
+      </c>
+      <c r="B15">
+        <v>704</v>
+      </c>
+      <c r="C15">
+        <v>448</v>
+      </c>
+      <c r="D15">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.05</v>
+      </c>
+      <c r="B16">
+        <v>699</v>
+      </c>
+      <c r="C16">
+        <v>517</v>
+      </c>
+      <c r="D16">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.04</v>
+      </c>
+      <c r="B17">
+        <v>690</v>
+      </c>
+      <c r="C17">
+        <v>623</v>
+      </c>
+      <c r="D17">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.03</v>
+      </c>
+      <c r="B18">
+        <v>681</v>
+      </c>
+      <c r="C18">
+        <v>792</v>
+      </c>
+      <c r="D18">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.02</v>
+      </c>
+      <c r="B19">
+        <v>707</v>
+      </c>
+      <c r="C19">
+        <v>1124</v>
+      </c>
+      <c r="D19">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.01</v>
+      </c>
+      <c r="B20">
+        <v>710</v>
+      </c>
+      <c r="C20">
+        <v>1999</v>
+      </c>
+      <c r="D20">
+        <v>1330</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More better documentation in the performance section. Also added std::unordered_set to the arena.
</commit_message>
<xml_diff>
--- a/tests/Performance results.xlsx
+++ b/tests/Performance results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="normal" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>sigma</t>
   </si>
@@ -43,9 +43,6 @@
     <t>so::vector&lt;move-to-front&gt;</t>
   </si>
   <si>
-    <t>param</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>so::vector&lt;transpose&gt;</t>
+  </si>
+  <si>
+    <t>std::unordered_set</t>
   </si>
 </sst>
 </file>
@@ -214,25 +214,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.3E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.2000000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.5E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>4.9000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -248,7 +248,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std::list</c:v>
+                  <c:v>std::unordered_set</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -293,25 +293,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>11.378</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.632</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.818</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.241</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.202999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.497999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.571999999999999</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,7 +327,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std::vector</c:v>
+                  <c:v>std::list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -372,25 +372,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.9369999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0209999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.9630000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.802</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.827</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.8210000000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.84</c:v>
+                  <c:v>11.122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.166</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.862</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.989000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -406,7 +406,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;count&gt;</c:v>
+                  <c:v>std::vector</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -451,25 +451,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>54.085999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41.878</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.771999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18.327999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.242000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.2910000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.2460000000000004</c:v>
+                  <c:v>3.7989999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7029999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9289999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6349999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -485,7 +485,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;transpose&gt;</c:v>
+                  <c:v>so::list&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,25 +530,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>11.423999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.204000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.444000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.212999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.215999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.117000000000001</c:v>
+                  <c:v>53.923000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.162000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,7 +564,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                  <c:v>so::list&lt;transpose&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -609,25 +609,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>47.075000000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35.542000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.239999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.122</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.8540000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.1139999999999999</c:v>
+                  <c:v>11.276</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.327999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.089</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.329000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.848000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,7 +643,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::vector&lt;count&gt;</c:v>
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -688,25 +688,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>55.220999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>56.359000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>54.023000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54.268999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>54.198999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54.587000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>54.194000000000003</c:v>
+                  <c:v>47.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.783000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.219000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.959</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.523999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,7 +722,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::vector&lt;transpose&gt;</c:v>
+                  <c:v>so::vector&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -767,25 +767,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.8639999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.92</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.8370000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.843</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.8620000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.827</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.8370000000000002</c:v>
+                  <c:v>53.536000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.213000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.817999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.514000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.959000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,7 +801,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::vector&lt;move-to-front&gt;</c:v>
+                  <c:v>so::vector&lt;transpose&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -846,25 +846,104 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>35.305</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>34.494999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33.44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32.822000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32.838000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.896999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32.622</c:v>
+                  <c:v>3.7469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.915</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1310000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>normal!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::vector&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>normal!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>normal!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>34.771999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.161000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.488999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.530999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.654000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.328000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1090,25 +1169,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.9000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.7E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.4999999999999998E-2</c:v>
+                  <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1124,7 +1203,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std::list</c:v>
+                  <c:v>std::unordered_set</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1169,25 +1248,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>11.887</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.209</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.212</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.839</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.592000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.558999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.135999999999999</c:v>
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1203,7 +1282,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>std::vector</c:v>
+                  <c:v>std::list</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1248,25 +1327,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.0179999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.8980000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.048</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.8260000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1749999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.8180000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7869999999999999</c:v>
+                  <c:v>11.430999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.798999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.927</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.678000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.827</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,7 +1361,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;count&gt;</c:v>
+                  <c:v>std::vector</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1327,25 +1406,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>56.33</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40.884999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.97</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18.146999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.667999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.1419999999999995</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0439999999999996</c:v>
+                  <c:v>4.0289999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7919999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8290000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6850000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1361,7 +1440,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;transpose&gt;</c:v>
+                  <c:v>so::list&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1406,25 +1485,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>11.587999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.715</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.677</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.677</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.624000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.289</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.954000000000001</c:v>
+                  <c:v>29.628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.103000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.617000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.117000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9539999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0709999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,7 +1519,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                  <c:v>so::list&lt;transpose&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1485,25 +1564,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>29.841000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.516999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.2110000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.7130000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.8650000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2370000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98799999999999999</c:v>
+                  <c:v>11.606999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.489000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.884</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.427</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1519,7 +1598,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::vector&lt;count&gt;</c:v>
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1564,25 +1643,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>54.564999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.441000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>57.148000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54.430999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>53.585999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>53.823999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>54.33</c:v>
+                  <c:v>8.7780000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7789999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88800000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1598,7 +1677,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::vector&lt;transpose&gt;</c:v>
+                  <c:v>so::vector&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1643,25 +1722,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.883</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9279999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.8969999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.7370000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7549999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7480000000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.7410000000000001</c:v>
+                  <c:v>51.725999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.975000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.264000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.654000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,7 +1756,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::vector&lt;move-to-front&gt;</c:v>
+                  <c:v>so::vector&lt;transpose&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1722,25 +1801,104 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>33.569000000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33.481999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35.371000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.941000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33.081000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33.090000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32.238999999999997</c:v>
+                  <c:v>3.7440000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.758</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7549999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'normal, sorted'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::vector&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'normal, sorted'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'normal, sorted'!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>32.146999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.587</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.097999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.231999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.242999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.701000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1937,65 +2095,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'geometric, 100000'!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
+              <c:f>'geometric, 100000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2003,66 +2158,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'geometric, 100000'!$B$2:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="2">
+              <c:f>'geometric, 100000'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2078,7 +2230,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;count&gt;</c:v>
+                  <c:v>std::unordered_set</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2088,65 +2240,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'geometric, 100000'!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
+              <c:f>'geometric, 100000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2154,66 +2303,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'geometric, 100000'!$C$2:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18</c:v>
+              <c:f>'geometric, 100000'!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>26</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>37</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>39</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>53</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>65</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>82</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>104</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>269</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,7 +2375,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                  <c:v>so::list&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2239,65 +2385,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'geometric, 100000'!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
+              <c:f>'geometric, 100000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2305,66 +2448,208 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'geometric, 100000'!$D$2:$D$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
+              <c:f>'geometric, 100000'!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>246</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 100000'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 100000'!$E$2:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>59</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>69</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>176</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2519,7 +2804,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>search 100000 geometrically distributed integers in, by </a:t>
+              <a:t>search 100000 geometrically distributed integers, by </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" i="1" baseline="0">
@@ -2561,65 +2846,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'geometric, 1000000'!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
+              <c:f>'geometric, 1000000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2627,66 +2909,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'geometric, 1000000'!$B$2:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>687</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>692</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>669</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>689</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>682</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>743</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>704</c:v>
+              <c:f>'geometric, 1000000'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>697</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>702</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>679</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>700</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>700</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>721</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>704</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>699</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>690</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>681</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>707</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>710</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2702,7 +2981,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;count&gt;</c:v>
+                  <c:v>std::unordered_set</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2712,65 +2991,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'geometric, 1000000'!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
+              <c:f>'geometric, 1000000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2778,66 +3054,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'geometric, 1000000'!$C$2:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>133</c:v>
+              <c:f>'geometric, 1000000'!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>135</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>184</c:v>
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>282</c:v>
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>308</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>362</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>399</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>517</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>623</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>792</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>1124</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1999</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2853,7 +3126,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                  <c:v>so::list&lt;count&gt;</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2863,65 +3136,62 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'geometric, 1000000'!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
+              <c:f>'geometric, 1000000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.06</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.04</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -2929,66 +3199,208 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'geometric, 1000000'!$D$2:$D$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
+              <c:f>'geometric, 1000000'!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'geometric, 1000000'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>so::list&lt;move-to-front&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'geometric, 1000000'!$E$2:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>117</c:v>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>119</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>156</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>214</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>235</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>257</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>292</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>326</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>369</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>444</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>574</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>747</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1330</c:v>
+                  <c:v>232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3115,7 +3527,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>857250</xdr:colOff>
+      <xdr:colOff>948690</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
@@ -3152,7 +3564,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>868680</xdr:colOff>
+      <xdr:colOff>960120</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -3183,15 +3595,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>331470</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3217,16 +3629,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>80010</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>384810</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3535,26 +3947,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3562,252 +3976,276 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15000</v>
       </c>
       <c r="B2">
-        <v>6.3E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C2">
-        <v>11.378</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D2">
-        <v>3.9369999999999998</v>
+        <v>11.122</v>
       </c>
       <c r="E2">
-        <v>54.085999999999999</v>
+        <v>3.7989999999999999</v>
       </c>
       <c r="F2">
-        <v>11.423999999999999</v>
+        <v>53.923000000000002</v>
       </c>
       <c r="G2">
-        <v>47.075000000000003</v>
+        <v>11.276</v>
       </c>
       <c r="H2">
-        <v>55.220999999999997</v>
+        <v>47.91</v>
       </c>
       <c r="I2">
-        <v>3.8639999999999999</v>
+        <v>53.536000000000001</v>
       </c>
       <c r="J2">
-        <v>35.305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.7469999999999999</v>
+      </c>
+      <c r="K2">
+        <v>34.771999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>8.2000000000000003E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C3">
-        <v>11.632</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D3">
-        <v>4.0209999999999999</v>
+        <v>10.869</v>
       </c>
       <c r="E3">
-        <v>41.878</v>
+        <v>3.7029999999999998</v>
       </c>
       <c r="F3">
-        <v>11.78</v>
+        <v>41.363</v>
       </c>
       <c r="G3">
-        <v>35.542000000000002</v>
+        <v>11.327999999999999</v>
       </c>
       <c r="H3">
-        <v>56.359000000000002</v>
+        <v>34.783000000000001</v>
       </c>
       <c r="I3">
-        <v>3.92</v>
+        <v>54.213000000000001</v>
       </c>
       <c r="J3">
-        <v>34.494999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="K3">
+        <v>33.161000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5000</v>
       </c>
       <c r="B4">
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C4">
-        <v>11.818</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D4">
-        <v>3.9630000000000001</v>
+        <v>11.166</v>
       </c>
       <c r="E4">
-        <v>22.771999999999998</v>
+        <v>3.8010000000000002</v>
       </c>
       <c r="F4">
-        <v>11.204000000000001</v>
+        <v>22.42</v>
       </c>
       <c r="G4">
-        <v>20.009</v>
+        <v>11.089</v>
       </c>
       <c r="H4">
-        <v>54.023000000000003</v>
+        <v>20.219000000000001</v>
       </c>
       <c r="I4">
-        <v>3.8370000000000002</v>
+        <v>55.09</v>
       </c>
       <c r="J4">
-        <v>33.44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.915</v>
+      </c>
+      <c r="K4">
+        <v>33.488999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4000</v>
       </c>
       <c r="B5">
-        <v>0.06</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="C5">
-        <v>11.241</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D5">
-        <v>3.802</v>
+        <v>12.776</v>
       </c>
       <c r="E5">
-        <v>18.327999999999999</v>
+        <v>3.9289999999999998</v>
       </c>
       <c r="F5">
-        <v>11.444000000000001</v>
+        <v>18.506</v>
       </c>
       <c r="G5">
-        <v>16.239999999999998</v>
+        <v>11.064</v>
       </c>
       <c r="H5">
-        <v>54.268999999999998</v>
+        <v>15.959</v>
       </c>
       <c r="I5">
-        <v>3.843</v>
+        <v>54.695999999999998</v>
       </c>
       <c r="J5">
-        <v>32.822000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.0279999999999996</v>
+      </c>
+      <c r="K5">
+        <v>32.530999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3000</v>
       </c>
       <c r="B6">
-        <v>5.7000000000000002E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C6">
-        <v>11.202999999999999</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D6">
-        <v>3.827</v>
+        <v>12.231</v>
       </c>
       <c r="E6">
-        <v>14.242000000000001</v>
+        <v>4.12</v>
       </c>
       <c r="F6">
-        <v>11.212999999999999</v>
+        <v>14.162000000000001</v>
       </c>
       <c r="G6">
-        <v>12.122</v>
+        <v>11.329000000000001</v>
       </c>
       <c r="H6">
-        <v>54.198999999999998</v>
+        <v>12.523999999999999</v>
       </c>
       <c r="I6">
-        <v>3.8620000000000001</v>
+        <v>54.817999999999998</v>
       </c>
       <c r="J6">
-        <v>32.838000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>4.1310000000000002</v>
+      </c>
+      <c r="K6">
+        <v>33.654000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2000</v>
       </c>
       <c r="B7">
-        <v>5.5E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C7">
-        <v>11.497999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="D7">
-        <v>3.8210000000000002</v>
+        <v>11.862</v>
       </c>
       <c r="E7">
-        <v>9.2910000000000004</v>
+        <v>3.96</v>
       </c>
       <c r="F7">
-        <v>11.215999999999999</v>
+        <v>9.0250000000000004</v>
       </c>
       <c r="G7">
-        <v>7.8540000000000001</v>
+        <v>10.848000000000001</v>
       </c>
       <c r="H7">
-        <v>54.587000000000003</v>
+        <v>8.125</v>
       </c>
       <c r="I7">
-        <v>3.827</v>
+        <v>53.514000000000003</v>
       </c>
       <c r="J7">
-        <v>32.896999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.9169999999999998</v>
+      </c>
+      <c r="K7">
+        <v>32.328000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1000</v>
       </c>
       <c r="B8">
-        <v>5.5E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C8">
-        <v>11.571999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="D8">
-        <v>3.84</v>
+        <v>10.989000000000001</v>
       </c>
       <c r="E8">
-        <v>4.2460000000000004</v>
+        <v>3.6349999999999998</v>
       </c>
       <c r="F8">
-        <v>11.117000000000001</v>
+        <v>4.165</v>
       </c>
       <c r="G8">
-        <v>3.1139999999999999</v>
+        <v>10.65</v>
       </c>
       <c r="H8">
-        <v>54.194000000000003</v>
+        <v>3.12</v>
       </c>
       <c r="I8">
-        <v>3.8370000000000002</v>
+        <v>52.959000000000003</v>
       </c>
       <c r="J8">
-        <v>32.622</v>
+        <v>3.6379999999999999</v>
+      </c>
+      <c r="K8">
+        <v>31.94</v>
       </c>
     </row>
   </sheetData>
@@ -3819,581 +4257,652 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15000</v>
       </c>
       <c r="B2">
-        <v>5.0999999999999997E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="C2">
-        <v>11.887</v>
+        <v>0.02</v>
       </c>
       <c r="D2">
-        <v>4.0179999999999998</v>
+        <v>11.430999999999999</v>
       </c>
       <c r="E2">
-        <v>56.33</v>
+        <v>4.0289999999999999</v>
       </c>
       <c r="F2">
-        <v>11.587999999999999</v>
+        <v>29.628</v>
       </c>
       <c r="G2">
-        <v>29.841000000000001</v>
+        <v>11.606999999999999</v>
       </c>
       <c r="H2">
-        <v>54.564999999999998</v>
+        <v>8.7780000000000005</v>
       </c>
       <c r="I2">
-        <v>3.883</v>
+        <v>51.725999999999999</v>
       </c>
       <c r="J2">
-        <v>33.569000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.7440000000000002</v>
+      </c>
+      <c r="K2">
+        <v>32.146999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>4.9000000000000002E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="C3">
-        <v>11.209</v>
+        <v>0.02</v>
       </c>
       <c r="D3">
-        <v>3.8980000000000001</v>
+        <v>10.798999999999999</v>
       </c>
       <c r="E3">
-        <v>40.884999999999998</v>
+        <v>3.7919999999999998</v>
       </c>
       <c r="F3">
-        <v>11.715</v>
+        <v>27.103000000000002</v>
       </c>
       <c r="G3">
-        <v>18.516999999999999</v>
+        <v>10.87</v>
       </c>
       <c r="H3">
-        <v>54.441000000000003</v>
+        <v>6.6</v>
       </c>
       <c r="I3">
-        <v>3.9279999999999999</v>
+        <v>53.975000000000001</v>
       </c>
       <c r="J3">
-        <v>33.481999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.6560000000000001</v>
+      </c>
+      <c r="K3">
+        <v>31.689</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5000</v>
       </c>
       <c r="B4">
-        <v>4.7E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C4">
-        <v>11.212</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D4">
-        <v>4.048</v>
+        <v>10.927</v>
       </c>
       <c r="E4">
-        <v>22.97</v>
+        <v>3.669</v>
       </c>
       <c r="F4">
-        <v>11.677</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="G4">
-        <v>8.2110000000000003</v>
+        <v>10.669</v>
       </c>
       <c r="H4">
-        <v>57.148000000000003</v>
+        <v>3.7290000000000001</v>
       </c>
       <c r="I4">
-        <v>3.8969999999999998</v>
+        <v>52.264000000000003</v>
       </c>
       <c r="J4">
-        <v>35.371000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.6669999999999998</v>
+      </c>
+      <c r="K4">
+        <v>31.587</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4000</v>
       </c>
       <c r="B5">
-        <v>0.05</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C5">
-        <v>11.839</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D5">
-        <v>3.8260000000000001</v>
+        <v>10.678000000000001</v>
       </c>
       <c r="E5">
-        <v>18.146999999999998</v>
+        <v>3.8290000000000002</v>
       </c>
       <c r="F5">
-        <v>11.677</v>
+        <v>15.617000000000001</v>
       </c>
       <c r="G5">
-        <v>5.7130000000000001</v>
+        <v>11.489000000000001</v>
       </c>
       <c r="H5">
-        <v>54.430999999999997</v>
+        <v>3.4039999999999999</v>
       </c>
       <c r="I5">
-        <v>3.7370000000000001</v>
+        <v>52.89</v>
       </c>
       <c r="J5">
-        <v>34.941000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.72</v>
+      </c>
+      <c r="K5">
+        <v>32.097999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3000</v>
       </c>
       <c r="B6">
-        <v>4.5999999999999999E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C6">
-        <v>11.592000000000001</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D6">
-        <v>4.1749999999999998</v>
+        <v>10.83</v>
       </c>
       <c r="E6">
-        <v>14.667999999999999</v>
+        <v>3.7229999999999999</v>
       </c>
       <c r="F6">
-        <v>11.624000000000001</v>
+        <v>12.117000000000001</v>
       </c>
       <c r="G6">
-        <v>3.8650000000000002</v>
+        <v>11.884</v>
       </c>
       <c r="H6">
-        <v>53.585999999999999</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="I6">
-        <v>3.7549999999999999</v>
+        <v>53.83</v>
       </c>
       <c r="J6">
-        <v>33.081000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.758</v>
+      </c>
+      <c r="K6">
+        <v>32.231999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2000</v>
       </c>
       <c r="B7">
-        <v>4.5999999999999999E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>11.558999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D7">
-        <v>3.8180000000000001</v>
+        <v>10.827</v>
       </c>
       <c r="E7">
-        <v>9.1419999999999995</v>
+        <v>3.7040000000000002</v>
       </c>
       <c r="F7">
-        <v>11.289</v>
+        <v>7.9539999999999997</v>
       </c>
       <c r="G7">
-        <v>2.2370000000000001</v>
+        <v>11.427</v>
       </c>
       <c r="H7">
-        <v>53.823999999999998</v>
+        <v>1.7789999999999999</v>
       </c>
       <c r="I7">
-        <v>3.7480000000000002</v>
+        <v>52.654000000000003</v>
       </c>
       <c r="J7">
-        <v>33.090000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.7349999999999999</v>
+      </c>
+      <c r="K7">
+        <v>31.242999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1000</v>
       </c>
       <c r="B8">
-        <v>4.4999999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="C8">
-        <v>11.135999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D8">
-        <v>3.7869999999999999</v>
+        <v>11.07</v>
       </c>
       <c r="E8">
-        <v>4.0439999999999996</v>
+        <v>3.6850000000000001</v>
       </c>
       <c r="F8">
-        <v>10.954000000000001</v>
+        <v>4.0709999999999997</v>
       </c>
       <c r="G8">
-        <v>0.98799999999999999</v>
+        <v>11.04</v>
       </c>
       <c r="H8">
-        <v>54.33</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="I8">
-        <v>3.7410000000000001</v>
+        <v>53.381</v>
       </c>
       <c r="J8">
-        <v>32.238999999999997</v>
+        <v>3.7549999999999999</v>
+      </c>
+      <c r="K8">
+        <v>31.701000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="B2">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.8</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="E3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.7</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0.9</v>
-      </c>
-      <c r="B3">
-        <v>44</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.6</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.8</v>
-      </c>
-      <c r="B4">
-        <v>41</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <v>38</v>
+      </c>
+      <c r="C7">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0.7</v>
-      </c>
-      <c r="B5">
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.09</v>
+      </c>
+      <c r="B11">
+        <v>36</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.08</v>
+      </c>
+      <c r="B12">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12">
         <v>40</v>
       </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0.6</v>
-      </c>
-      <c r="B6">
-        <v>39</v>
-      </c>
-      <c r="C6">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0.5</v>
-      </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
-      </c>
-      <c r="D7">
+      <c r="E12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B13">
+        <v>37</v>
+      </c>
+      <c r="C13">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0.4</v>
-      </c>
-      <c r="B8">
-        <v>41</v>
-      </c>
-      <c r="C8">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0.3</v>
-      </c>
-      <c r="B9">
-        <v>41</v>
-      </c>
-      <c r="C9">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0.2</v>
-      </c>
-      <c r="B10">
-        <v>48</v>
-      </c>
-      <c r="C10">
-        <v>26</v>
-      </c>
-      <c r="D10">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0.1</v>
-      </c>
-      <c r="B11">
-        <v>45</v>
-      </c>
-      <c r="C11">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0.09</v>
-      </c>
-      <c r="B12">
-        <v>46</v>
-      </c>
-      <c r="C12">
-        <v>43</v>
-      </c>
-      <c r="D12">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>0.08</v>
-      </c>
-      <c r="B13">
-        <v>47</v>
-      </c>
-      <c r="C13">
-        <v>39</v>
       </c>
       <c r="D13">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="B14">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C14">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="B15">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="B16">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C16">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E16">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="B17">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="E17">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="B18">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="D18">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="E18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="B19">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="D19">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>0.01</v>
-      </c>
-      <c r="B20">
-        <v>47</v>
-      </c>
-      <c r="C20">
-        <v>269</v>
-      </c>
-      <c r="D20">
-        <v>176</v>
+        <v>246</v>
+      </c>
+      <c r="E19">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4404,298 +4913,342 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="B2">
-        <v>687</v>
+        <v>292</v>
       </c>
       <c r="C2">
+        <v>312</v>
+      </c>
+      <c r="D2">
+        <v>72</v>
+      </c>
+      <c r="E2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.8</v>
+      </c>
+      <c r="B3">
+        <v>289</v>
+      </c>
+      <c r="C3">
+        <v>341</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+      <c r="E3">
         <v>82</v>
       </c>
-      <c r="D2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.7</v>
+      </c>
+      <c r="B4">
+        <v>268</v>
+      </c>
+      <c r="C4">
+        <v>326</v>
+      </c>
+      <c r="D4">
+        <v>75</v>
+      </c>
+      <c r="E4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.6</v>
+      </c>
+      <c r="B5">
+        <v>266</v>
+      </c>
+      <c r="C5">
+        <v>306</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>257</v>
+      </c>
+      <c r="C6">
+        <v>316</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+      <c r="E6">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0.9</v>
-      </c>
-      <c r="B3">
-        <v>692</v>
-      </c>
-      <c r="C3">
-        <v>85</v>
-      </c>
-      <c r="D3">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.8</v>
-      </c>
-      <c r="B4">
-        <v>669</v>
-      </c>
-      <c r="C4">
-        <v>87</v>
-      </c>
-      <c r="D4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <v>264</v>
+      </c>
+      <c r="C7">
+        <v>312</v>
+      </c>
+      <c r="D7">
+        <v>75</v>
+      </c>
+      <c r="E7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8">
+        <v>262</v>
+      </c>
+      <c r="C8">
+        <v>313</v>
+      </c>
+      <c r="D8">
+        <v>81</v>
+      </c>
+      <c r="E8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>305</v>
+      </c>
+      <c r="D9">
+        <v>82</v>
+      </c>
+      <c r="E9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10">
+        <v>275</v>
+      </c>
+      <c r="C10">
+        <v>313</v>
+      </c>
+      <c r="D10">
+        <v>92</v>
+      </c>
+      <c r="E10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.09</v>
+      </c>
+      <c r="B11">
+        <v>272</v>
+      </c>
+      <c r="C11">
+        <v>313</v>
+      </c>
+      <c r="D11">
+        <v>96</v>
+      </c>
+      <c r="E11">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.08</v>
+      </c>
+      <c r="B12">
+        <v>269</v>
+      </c>
+      <c r="C12">
+        <v>306</v>
+      </c>
+      <c r="D12">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0.7</v>
-      </c>
-      <c r="B5">
-        <v>689</v>
-      </c>
-      <c r="C5">
-        <v>93</v>
-      </c>
-      <c r="D5">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0.6</v>
-      </c>
-      <c r="B6">
-        <v>682</v>
-      </c>
-      <c r="C6">
+      <c r="E12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B13">
+        <v>271</v>
+      </c>
+      <c r="C13">
+        <v>315</v>
+      </c>
+      <c r="D13">
+        <v>106</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.06</v>
+      </c>
+      <c r="B14">
+        <v>267</v>
+      </c>
+      <c r="C14">
+        <v>310</v>
+      </c>
+      <c r="D14">
         <v>107</v>
       </c>
-      <c r="D6">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0.5</v>
-      </c>
-      <c r="B7">
-        <v>743</v>
-      </c>
-      <c r="C7">
-        <v>122</v>
-      </c>
-      <c r="D7">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0.4</v>
-      </c>
-      <c r="B8">
-        <v>704</v>
-      </c>
-      <c r="C8">
+      <c r="E14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.05</v>
+      </c>
+      <c r="B15">
+        <v>267</v>
+      </c>
+      <c r="C15">
+        <v>312</v>
+      </c>
+      <c r="D15">
+        <v>128</v>
+      </c>
+      <c r="E15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.04</v>
+      </c>
+      <c r="B16">
+        <v>278</v>
+      </c>
+      <c r="C16">
+        <v>312</v>
+      </c>
+      <c r="D16">
         <v>133</v>
       </c>
-      <c r="D8">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0.3</v>
-      </c>
-      <c r="B9">
-        <v>697</v>
-      </c>
-      <c r="C9">
-        <v>135</v>
-      </c>
-      <c r="D9">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0.2</v>
-      </c>
-      <c r="B10">
-        <v>702</v>
-      </c>
-      <c r="C10">
-        <v>184</v>
-      </c>
-      <c r="D10">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0.1</v>
-      </c>
-      <c r="B11">
-        <v>679</v>
-      </c>
-      <c r="C11">
-        <v>282</v>
-      </c>
-      <c r="D11">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0.09</v>
-      </c>
-      <c r="B12">
-        <v>700</v>
-      </c>
-      <c r="C12">
+      <c r="E16">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.03</v>
+      </c>
+      <c r="B17">
+        <v>266</v>
+      </c>
+      <c r="C17">
+        <v>307</v>
+      </c>
+      <c r="D17">
+        <v>148</v>
+      </c>
+      <c r="E17">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.02</v>
+      </c>
+      <c r="B18">
+        <v>273</v>
+      </c>
+      <c r="C18">
         <v>308</v>
       </c>
-      <c r="D12">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>0.08</v>
-      </c>
-      <c r="B13">
-        <v>700</v>
-      </c>
-      <c r="C13">
-        <v>362</v>
-      </c>
-      <c r="D13">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="B14">
-        <v>721</v>
-      </c>
-      <c r="C14">
-        <v>399</v>
-      </c>
-      <c r="D14">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>0.06</v>
-      </c>
-      <c r="B15">
-        <v>704</v>
-      </c>
-      <c r="C15">
-        <v>448</v>
-      </c>
-      <c r="D15">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>0.05</v>
-      </c>
-      <c r="B16">
-        <v>699</v>
-      </c>
-      <c r="C16">
-        <v>517</v>
-      </c>
-      <c r="D16">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>0.04</v>
-      </c>
-      <c r="B17">
-        <v>690</v>
-      </c>
-      <c r="C17">
-        <v>623</v>
-      </c>
-      <c r="D17">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>0.03</v>
-      </c>
-      <c r="B18">
-        <v>681</v>
-      </c>
-      <c r="C18">
-        <v>792</v>
-      </c>
       <c r="D18">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="E18">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="B19">
-        <v>707</v>
+        <v>268</v>
       </c>
       <c r="C19">
-        <v>1124</v>
+        <v>316</v>
       </c>
       <c r="D19">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>0.01</v>
-      </c>
-      <c r="B20">
-        <v>710</v>
-      </c>
-      <c r="C20">
-        <v>1999</v>
-      </c>
-      <c r="D20">
-        <v>1330</v>
+        <v>304</v>
+      </c>
+      <c r="E19">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted year of copyright. Added LICENSE and README files in preparation for GitHub push.
</commit_message>
<xml_diff>
--- a/tests/Performance results.xlsx
+++ b/tests/Performance results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="normal" sheetId="1" r:id="rId1"/>
@@ -4259,7 +4259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -4915,7 +4915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>